<commit_message>
Notebook: now agents have upstream and downstream
</commit_message>
<xml_diff>
--- a/Beerhouse/aux_documents/creating_consumer_trend.xlsx
+++ b/Beerhouse/aux_documents/creating_consumer_trend.xlsx
@@ -424,40 +424,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>33.5669</c:v>
+                  <c:v>35.1579</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.4691</c:v>
+                  <c:v>30.9556</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.2604</c:v>
+                  <c:v>35.84840000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.6175</c:v>
+                  <c:v>31.8893</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.0581</c:v>
+                  <c:v>34.6097</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.73780000000001</c:v>
+                  <c:v>33.9613</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.2468</c:v>
+                  <c:v>34.1274</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.2824</c:v>
+                  <c:v>33.5465</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.8283</c:v>
+                  <c:v>38.62039999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.3069</c:v>
+                  <c:v>35.59469999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.4054</c:v>
+                  <c:v>32.6426</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.16150000000001</c:v>
+                  <c:v>50.2171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,25 +613,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.98</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.966</c:v>
+                  <c:v>0.943</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9102</c:v>
+                  <c:v>0.9546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0332</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2284</c:v>
+                  <c:v>1.3172</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3855</c:v>
+                  <c:v>1.5811</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9758</c:v>
+                  <c:v>1.0472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,25 +680,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.78</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0235</c:v>
+                  <c:v>0.966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0212</c:v>
+                  <c:v>1.0101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2474</c:v>
+                  <c:v>0.9954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.406</c:v>
+                  <c:v>1.2876</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2388</c:v>
+                  <c:v>1.4833</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9758</c:v>
+                  <c:v>1.0829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,25 +747,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.87</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0005</c:v>
+                  <c:v>1.012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9435</c:v>
+                  <c:v>0.9768</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1466</c:v>
+                  <c:v>1.197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1988</c:v>
+                  <c:v>1.406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3529</c:v>
+                  <c:v>1.4344</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0234</c:v>
+                  <c:v>1.0948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -814,25 +814,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.86</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.104</c:v>
+                  <c:v>0.9545</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9657</c:v>
+                  <c:v>1.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2222</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4208</c:v>
+                  <c:v>1.11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4996</c:v>
+                  <c:v>1.63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1662</c:v>
+                  <c:v>0.9282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,25 +881,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.84</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.943</c:v>
+                  <c:v>1.1155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8436</c:v>
+                  <c:v>0.8991</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1718</c:v>
+                  <c:v>1.0332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4652</c:v>
+                  <c:v>1.184</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3855</c:v>
+                  <c:v>1.5159</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9401</c:v>
+                  <c:v>1.1781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,25 +948,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.966</c:v>
+                  <c:v>1.0465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9102</c:v>
+                  <c:v>0.8547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1592</c:v>
+                  <c:v>1.134</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.184</c:v>
+                  <c:v>1.4652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2551</c:v>
+                  <c:v>1.5974</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1424</c:v>
+                  <c:v>1.0948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,25 +1015,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9213</c:v>
+                  <c:v>0.8769</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.071</c:v>
+                  <c:v>1.0584</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.11</c:v>
+                  <c:v>1.4652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6137</c:v>
+                  <c:v>1.3692</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1424</c:v>
+                  <c:v>0.8925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,25 +1082,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9775</c:v>
+                  <c:v>0.897</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0878</c:v>
+                  <c:v>0.9102</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1592</c:v>
+                  <c:v>0.945</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.184</c:v>
+                  <c:v>1.1248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4181</c:v>
+                  <c:v>1.2225</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9877</c:v>
+                  <c:v>1.1186</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,25 +1149,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.88</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9315</c:v>
+                  <c:v>1.1385</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0212</c:v>
+                  <c:v>0.8658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1466</c:v>
+                  <c:v>1.1088</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.304</c:v>
+                  <c:v>1.4344</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1662</c:v>
+                  <c:v>0.9758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,25 +1216,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.96</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9315</c:v>
+                  <c:v>1.0695</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9546</c:v>
+                  <c:v>0.8436</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9576</c:v>
+                  <c:v>1.2474</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.332</c:v>
+                  <c:v>1.4208</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5485</c:v>
+                  <c:v>1.5648</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.071</c:v>
+                  <c:v>1.1662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,25 +1283,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.99</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0235</c:v>
+                  <c:v>1.035</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.999</c:v>
+                  <c:v>0.8547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0962</c:v>
+                  <c:v>1.0836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1988</c:v>
+                  <c:v>1.1692</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4507</c:v>
+                  <c:v>1.5159</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9163</c:v>
+                  <c:v>1.1662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1350,25 +1350,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.83</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.897</c:v>
+                  <c:v>0.8855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8325</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1592</c:v>
+                  <c:v>1.0458</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3616</c:v>
+                  <c:v>1.1692</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5811</c:v>
+                  <c:v>1.4507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1305</c:v>
+                  <c:v>1.1424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4747,7 +4747,7 @@
   <dimension ref="A1:AK14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6544,111 +6544,111 @@
       </c>
       <c r="B3" s="5">
         <f ca="1">'base behaviour'!B3*RANDBETWEEN(75,100)/100</f>
-        <v>1.56</v>
+        <v>1.8</v>
       </c>
       <c r="C3" s="5">
         <f ca="1">'base behaviour'!C3*RANDBETWEEN(75,100)/100</f>
-        <v>1.0580000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="D3" s="5">
         <f ca="1">'base behaviour'!D3*RANDBETWEEN(75,100)/100</f>
-        <v>0.94350000000000012</v>
+        <v>0.97680000000000011</v>
       </c>
       <c r="E3" s="5">
         <f ca="1">'base behaviour'!E3*RANDBETWEEN(75,100)/100</f>
-        <v>0.94499999999999995</v>
+        <v>1.2473999999999998</v>
       </c>
       <c r="F3" s="5">
         <f ca="1">'base behaviour'!F3*RANDBETWEEN(75,100)/100</f>
-        <v>1.258</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="G3" s="5">
         <f ca="1">'base behaviour'!G3*RANDBETWEEN(75,100)/100</f>
-        <v>1.2550999999999999</v>
+        <v>1.4506999999999999</v>
       </c>
       <c r="H3" s="5">
         <f ca="1">'base behaviour'!H3*RANDBETWEEN(75,100)/100</f>
-        <v>1.0471999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">'base behaviour'!I3*RANDBETWEEN(75,100)/100</f>
-        <v>0.98</v>
+        <v>0.83</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">'base behaviour'!J3*RANDBETWEEN(75,100)/100</f>
-        <v>0.96599999999999997</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="K3" s="5">
         <f ca="1">'base behaviour'!K3*RANDBETWEEN(75,100)/100</f>
-        <v>0.91020000000000012</v>
+        <v>0.95460000000000012</v>
       </c>
       <c r="L3" s="5">
         <f ca="1">'base behaviour'!L3*RANDBETWEEN(75,100)/100</f>
-        <v>1.0332000000000001</v>
+        <v>1.26</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">'base behaviour'!M3*RANDBETWEEN(75,100)/100</f>
-        <v>1.2283999999999999</v>
+        <v>1.3171999999999999</v>
       </c>
       <c r="N3" s="5">
         <f ca="1">'base behaviour'!N3*RANDBETWEEN(75,100)/100</f>
-        <v>1.3854999999999997</v>
+        <v>1.5810999999999999</v>
       </c>
       <c r="O3" s="5">
         <f ca="1">'base behaviour'!O3*RANDBETWEEN(75,100)/100</f>
-        <v>0.9758</v>
+        <v>1.0471999999999999</v>
       </c>
       <c r="P3" s="5">
         <f ca="1">'base behaviour'!P3*RANDBETWEEN(75,100)/100</f>
-        <v>0.95</v>
+        <v>0.81</v>
       </c>
       <c r="Q3" s="5">
         <f ca="1">'base behaviour'!Q3*RANDBETWEEN(75,100)/100</f>
-        <v>1.1039999999999999</v>
+        <v>1.081</v>
       </c>
       <c r="R3" s="5">
         <f ca="1">'base behaviour'!R3*RANDBETWEEN(75,100)/100</f>
-        <v>0.83250000000000013</v>
+        <v>0.93240000000000012</v>
       </c>
       <c r="S3" s="5">
         <f ca="1">'base behaviour'!S3*RANDBETWEEN(75,100)/100</f>
-        <v>1.2096</v>
+        <v>1.1214</v>
       </c>
       <c r="T3" s="5">
         <f ca="1">'base behaviour'!T3*RANDBETWEEN(75,100)/100</f>
-        <v>1.1395999999999999</v>
+        <v>1.2431999999999999</v>
       </c>
       <c r="U3" s="5">
         <f ca="1">'base behaviour'!U3*RANDBETWEEN(75,100)/100</f>
-        <v>1.5159</v>
+        <v>1.4832999999999998</v>
       </c>
       <c r="V3" s="5">
         <f ca="1">'base behaviour'!V3*RANDBETWEEN(75,100)/100</f>
-        <v>1.1305000000000001</v>
+        <v>0.96389999999999998</v>
       </c>
       <c r="W3" s="5">
         <f ca="1">'base behaviour'!W3*RANDBETWEEN(75,100)/100</f>
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="X3" s="5">
         <f ca="1">'base behaviour'!X3*RANDBETWEEN(75,100)/100</f>
-        <v>1.081</v>
+        <v>0.92</v>
       </c>
       <c r="Y3" s="5">
         <f ca="1">'base behaviour'!Y3*RANDBETWEEN(75,100)/100</f>
-        <v>0.92130000000000012</v>
+        <v>0.95460000000000012</v>
       </c>
       <c r="Z3" s="5">
         <f ca="1">'base behaviour'!Z3*RANDBETWEEN(75,100)/100</f>
-        <v>1.0835999999999999</v>
+        <v>1.1718000000000002</v>
       </c>
       <c r="AA3" s="5">
         <f ca="1">'base behaviour'!AA3*RANDBETWEEN(75,100)/100</f>
-        <v>1.2283999999999999</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="AB3" s="5">
         <f ca="1">'base behaviour'!AB3*RANDBETWEEN(75,100)/100</f>
-        <v>1.4017999999999997</v>
+        <v>1.3039999999999998</v>
       </c>
       <c r="AC3" s="5">
         <f ca="1">'base behaviour'!AC3*RANDBETWEEN(75,100)/100</f>
@@ -6656,15 +6656,15 @@
       </c>
       <c r="AD3" s="5">
         <f ca="1">'base behaviour'!AD3*RANDBETWEEN(75,100)/100</f>
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="AE3" s="5">
         <f ca="1">'base behaviour'!AE3*RANDBETWEEN(75,100)/100</f>
-        <v>0.98899999999999988</v>
+        <v>1.0234999999999999</v>
       </c>
       <c r="AF3" s="5">
         <f ca="1">'base behaviour'!AF3*RANDBETWEEN(75,100)/100</f>
-        <v>0.85470000000000013</v>
+        <v>0.96570000000000011</v>
       </c>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
@@ -6673,7 +6673,7 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="5">
         <f ca="1">SUM(B3:AK3)</f>
-        <v>33.566900000000004</v>
+        <v>35.157899999999991</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -6685,15 +6685,15 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5">
         <f ca="1">'base behaviour'!E4*RANDBETWEEN(75,100)/100</f>
-        <v>1.1088</v>
+        <v>1.1970000000000001</v>
       </c>
       <c r="F4" s="5">
         <f ca="1">'base behaviour'!F4*RANDBETWEEN(75,100)/100</f>
-        <v>1.2875999999999999</v>
+        <v>1.1840000000000002</v>
       </c>
       <c r="G4" s="5">
         <f ca="1">'base behaviour'!G4*RANDBETWEEN(75,100)/100</f>
-        <v>1.2387999999999999</v>
+        <v>1.5648</v>
       </c>
       <c r="H4" s="5">
         <f ca="1">'base behaviour'!H4*RANDBETWEEN(75,100)/100</f>
@@ -6701,99 +6701,99 @@
       </c>
       <c r="I4" s="5">
         <f ca="1">'base behaviour'!I4*RANDBETWEEN(75,100)/100</f>
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">'base behaviour'!J4*RANDBETWEEN(75,100)/100</f>
-        <v>1.0234999999999999</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="K4" s="5">
         <f ca="1">'base behaviour'!K4*RANDBETWEEN(75,100)/100</f>
-        <v>1.0212000000000001</v>
+        <v>1.0101</v>
       </c>
       <c r="L4" s="5">
         <f ca="1">'base behaviour'!L4*RANDBETWEEN(75,100)/100</f>
-        <v>1.2473999999999998</v>
+        <v>0.99540000000000006</v>
       </c>
       <c r="M4" s="5">
         <f ca="1">'base behaviour'!M4*RANDBETWEEN(75,100)/100</f>
-        <v>1.4059999999999999</v>
+        <v>1.2875999999999999</v>
       </c>
       <c r="N4" s="5">
         <f ca="1">'base behaviour'!N4*RANDBETWEEN(75,100)/100</f>
-        <v>1.2387999999999999</v>
+        <v>1.4832999999999998</v>
       </c>
       <c r="O4" s="5">
         <f ca="1">'base behaviour'!O4*RANDBETWEEN(75,100)/100</f>
-        <v>0.9758</v>
+        <v>1.0829</v>
       </c>
       <c r="P4" s="5">
         <f ca="1">'base behaviour'!P4*RANDBETWEEN(75,100)/100</f>
-        <v>0.79</v>
+        <v>0.81</v>
       </c>
       <c r="Q4" s="5">
         <f ca="1">'base behaviour'!Q4*RANDBETWEEN(75,100)/100</f>
-        <v>1.0694999999999999</v>
+        <v>1.0234999999999999</v>
       </c>
       <c r="R4" s="5">
         <f ca="1">'base behaviour'!R4*RANDBETWEEN(75,100)/100</f>
-        <v>1.0656000000000001</v>
+        <v>1.0878000000000001</v>
       </c>
       <c r="S4" s="5">
         <f ca="1">'base behaviour'!S4*RANDBETWEEN(75,100)/100</f>
-        <v>1.1088</v>
+        <v>0.98280000000000001</v>
       </c>
       <c r="T4" s="5">
         <f ca="1">'base behaviour'!T4*RANDBETWEEN(75,100)/100</f>
-        <v>1.48</v>
+        <v>1.3912</v>
       </c>
       <c r="U4" s="5">
         <f ca="1">'base behaviour'!U4*RANDBETWEEN(75,100)/100</f>
-        <v>1.63</v>
+        <v>1.3692</v>
       </c>
       <c r="V4" s="5">
         <f ca="1">'base behaviour'!V4*RANDBETWEEN(75,100)/100</f>
-        <v>1.1067</v>
+        <v>1.1305000000000001</v>
       </c>
       <c r="W4" s="5">
         <f ca="1">'base behaviour'!W4*RANDBETWEEN(75,100)/100</f>
-        <v>0.97</v>
+        <v>0.86</v>
       </c>
       <c r="X4" s="5">
         <f ca="1">'base behaviour'!X4*RANDBETWEEN(75,100)/100</f>
-        <v>1.0465</v>
+        <v>1.1039999999999999</v>
       </c>
       <c r="Y4" s="5">
         <f ca="1">'base behaviour'!Y4*RANDBETWEEN(75,100)/100</f>
-        <v>0.94350000000000012</v>
+        <v>0.93240000000000012</v>
       </c>
       <c r="Z4" s="5">
         <f ca="1">'base behaviour'!Z4*RANDBETWEEN(75,100)/100</f>
-        <v>1.071</v>
+        <v>0.95760000000000001</v>
       </c>
       <c r="AA4" s="5">
         <f ca="1">'base behaviour'!AA4*RANDBETWEEN(75,100)/100</f>
-        <v>1.2431999999999999</v>
+        <v>1.3319999999999999</v>
       </c>
       <c r="AB4" s="5">
         <f ca="1">'base behaviour'!AB4*RANDBETWEEN(75,100)/100</f>
-        <v>1.63</v>
+        <v>1.3203</v>
       </c>
       <c r="AC4" s="5">
         <f ca="1">'base behaviour'!AC4*RANDBETWEEN(75,100)/100</f>
-        <v>1.19</v>
+        <v>1.0353000000000001</v>
       </c>
       <c r="AD4" s="5">
         <f ca="1">'base behaviour'!AD4*RANDBETWEEN(75,100)/100</f>
-        <v>0.94</v>
+        <v>0.99</v>
       </c>
       <c r="AE4" s="5">
         <f ca="1">'base behaviour'!AE4*RANDBETWEEN(75,100)/100</f>
-        <v>0.93149999999999988</v>
+        <v>0.97749999999999981</v>
       </c>
       <c r="AF4" s="5">
         <f ca="1">'base behaviour'!AF4*RANDBETWEEN(75,100)/100</f>
-        <v>0.86580000000000013</v>
+        <v>0.92130000000000012</v>
       </c>
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
@@ -6802,7 +6802,7 @@
       <c r="AK4" s="5"/>
       <c r="AL4" s="5">
         <f ca="1">SUM(B4:AK4)</f>
-        <v>31.469100000000001</v>
+        <v>30.955599999999997</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -6814,91 +6814,91 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5">
         <f ca="1">'base behaviour'!E5*RANDBETWEEN(75,100)/100</f>
-        <v>1.0584</v>
+        <v>1.2096</v>
       </c>
       <c r="F5" s="5">
         <f ca="1">'base behaviour'!F5*RANDBETWEEN(75,100)/100</f>
-        <v>1.3468</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="G5" s="5">
         <f ca="1">'base behaviour'!G5*RANDBETWEEN(75,100)/100</f>
-        <v>1.2713999999999999</v>
+        <v>1.5648</v>
       </c>
       <c r="H5" s="5">
         <f ca="1">'base behaviour'!H5*RANDBETWEEN(75,100)/100</f>
-        <v>1.0829</v>
+        <v>1.1186</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">'base behaviour'!I5*RANDBETWEEN(75,100)/100</f>
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">'base behaviour'!J5*RANDBETWEEN(75,100)/100</f>
-        <v>1.0004999999999999</v>
+        <v>1.0119999999999998</v>
       </c>
       <c r="K5" s="5">
         <f ca="1">'base behaviour'!K5*RANDBETWEEN(75,100)/100</f>
-        <v>0.94350000000000012</v>
+        <v>0.97680000000000011</v>
       </c>
       <c r="L5" s="5">
         <f ca="1">'base behaviour'!L5*RANDBETWEEN(75,100)/100</f>
-        <v>1.1466000000000001</v>
+        <v>1.1970000000000001</v>
       </c>
       <c r="M5" s="5">
         <f ca="1">'base behaviour'!M5*RANDBETWEEN(75,100)/100</f>
-        <v>1.1987999999999999</v>
+        <v>1.4059999999999999</v>
       </c>
       <c r="N5" s="5">
         <f ca="1">'base behaviour'!N5*RANDBETWEEN(75,100)/100</f>
-        <v>1.3529</v>
+        <v>1.4343999999999999</v>
       </c>
       <c r="O5" s="5">
         <f ca="1">'base behaviour'!O5*RANDBETWEEN(75,100)/100</f>
-        <v>1.0233999999999999</v>
+        <v>1.0948</v>
       </c>
       <c r="P5" s="5">
         <f ca="1">'base behaviour'!P5*RANDBETWEEN(75,100)/100</f>
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="Q5" s="5">
         <f ca="1">'base behaviour'!Q5*RANDBETWEEN(75,100)/100</f>
-        <v>0.89699999999999991</v>
+        <v>1.0924999999999998</v>
       </c>
       <c r="R5" s="5">
         <f ca="1">'base behaviour'!R5*RANDBETWEEN(75,100)/100</f>
-        <v>1.0767000000000002</v>
+        <v>0.89910000000000012</v>
       </c>
       <c r="S5" s="5">
         <f ca="1">'base behaviour'!S5*RANDBETWEEN(75,100)/100</f>
-        <v>0.98280000000000001</v>
+        <v>1.071</v>
       </c>
       <c r="T5" s="5">
         <f ca="1">'base behaviour'!T5*RANDBETWEEN(75,100)/100</f>
-        <v>1.2727999999999999</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="U5" s="5">
         <f ca="1">'base behaviour'!U5*RANDBETWEEN(75,100)/100</f>
-        <v>1.6136999999999997</v>
+        <v>1.4832999999999998</v>
       </c>
       <c r="V5" s="5">
         <f ca="1">'base behaviour'!V5*RANDBETWEEN(75,100)/100</f>
-        <v>1.1542999999999999</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="W5" s="5">
         <f ca="1">'base behaviour'!W5*RANDBETWEEN(75,100)/100</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="X5" s="5">
         <f ca="1">'base behaviour'!X5*RANDBETWEEN(75,100)/100</f>
-        <v>0.92</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="Y5" s="5">
         <f ca="1">'base behaviour'!Y5*RANDBETWEEN(75,100)/100</f>
-        <v>0.95460000000000012</v>
+        <v>0.92130000000000012</v>
       </c>
       <c r="Z5" s="5">
         <f ca="1">'base behaviour'!Z5*RANDBETWEEN(75,100)/100</f>
-        <v>0.98280000000000001</v>
+        <v>1.2096</v>
       </c>
       <c r="AA5" s="5">
         <f ca="1">'base behaviour'!AA5*RANDBETWEEN(75,100)/100</f>
@@ -6906,41 +6906,41 @@
       </c>
       <c r="AB5" s="5">
         <f ca="1">'base behaviour'!AB5*RANDBETWEEN(75,100)/100</f>
-        <v>1.2224999999999999</v>
+        <v>1.3203</v>
       </c>
       <c r="AC5" s="5">
         <f ca="1">'base behaviour'!AC5*RANDBETWEEN(75,100)/100</f>
-        <v>1.1305000000000001</v>
+        <v>0.9758</v>
       </c>
       <c r="AD5" s="5">
         <f ca="1">'base behaviour'!AD5*RANDBETWEEN(75,100)/100</f>
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="AE5" s="5">
         <f ca="1">'base behaviour'!AE5*RANDBETWEEN(75,100)/100</f>
-        <v>0.92</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="AF5" s="5">
         <f ca="1">'base behaviour'!AF5*RANDBETWEEN(75,100)/100</f>
-        <v>0.94350000000000012</v>
+        <v>0.93240000000000012</v>
       </c>
       <c r="AG5" s="5">
         <f ca="1">'base behaviour'!AG5*RANDBETWEEN(75,100)/100</f>
-        <v>1.1718000000000002</v>
+        <v>1.2348000000000001</v>
       </c>
       <c r="AH5" s="5">
         <f ca="1">'base behaviour'!AH5*RANDBETWEEN(75,100)/100</f>
-        <v>1.3912</v>
+        <v>1.3615999999999999</v>
       </c>
       <c r="AI5" s="5">
         <f ca="1">'base behaviour'!AI5*RANDBETWEEN(75,100)/100</f>
-        <v>1.4669999999999999</v>
+        <v>1.5648</v>
       </c>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
       <c r="AL5" s="5">
         <f ca="1">SUM(B5:AK5)</f>
-        <v>34.260400000000004</v>
+        <v>35.848400000000005</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -6955,43 +6955,43 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5">
         <f ca="1">'base behaviour'!H6*RANDBETWEEN(75,100)/100</f>
-        <v>1.0233999999999999</v>
+        <v>0.94009999999999994</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">'base behaviour'!I6*RANDBETWEEN(75,100)/100</f>
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">'base behaviour'!J6*RANDBETWEEN(75,100)/100</f>
-        <v>1.1039999999999999</v>
+        <v>0.9544999999999999</v>
       </c>
       <c r="K6" s="5">
         <f ca="1">'base behaviour'!K6*RANDBETWEEN(75,100)/100</f>
-        <v>0.96570000000000011</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="L6" s="5">
         <f ca="1">'base behaviour'!L6*RANDBETWEEN(75,100)/100</f>
-        <v>1.2222</v>
+        <v>1.26</v>
       </c>
       <c r="M6" s="5">
         <f ca="1">'base behaviour'!M6*RANDBETWEEN(75,100)/100</f>
-        <v>1.4207999999999998</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="N6" s="5">
         <f ca="1">'base behaviour'!N6*RANDBETWEEN(75,100)/100</f>
-        <v>1.4995999999999998</v>
+        <v>1.63</v>
       </c>
       <c r="O6" s="5">
         <f ca="1">'base behaviour'!O6*RANDBETWEEN(75,100)/100</f>
-        <v>1.1661999999999999</v>
+        <v>0.92819999999999991</v>
       </c>
       <c r="P6" s="5">
         <f ca="1">'base behaviour'!P6*RANDBETWEEN(75,100)/100</f>
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="Q6" s="5">
         <f ca="1">'base behaviour'!Q6*RANDBETWEEN(75,100)/100</f>
-        <v>0.94299999999999995</v>
+        <v>1.081</v>
       </c>
       <c r="R6" s="5">
         <f ca="1">'base behaviour'!R6*RANDBETWEEN(75,100)/100</f>
@@ -6999,23 +6999,23 @@
       </c>
       <c r="S6" s="5">
         <f ca="1">'base behaviour'!S6*RANDBETWEEN(75,100)/100</f>
-        <v>0.94499999999999995</v>
+        <v>1.2222</v>
       </c>
       <c r="T6" s="5">
         <f ca="1">'base behaviour'!T6*RANDBETWEEN(75,100)/100</f>
-        <v>1.1248</v>
+        <v>1.258</v>
       </c>
       <c r="U6" s="5">
         <f ca="1">'base behaviour'!U6*RANDBETWEEN(75,100)/100</f>
-        <v>1.4669999999999999</v>
+        <v>1.3854999999999997</v>
       </c>
       <c r="V6" s="5">
         <f ca="1">'base behaviour'!V6*RANDBETWEEN(75,100)/100</f>
-        <v>1.0114999999999998</v>
+        <v>1.0471999999999999</v>
       </c>
       <c r="W6" s="5">
         <f ca="1">'base behaviour'!W6*RANDBETWEEN(75,100)/100</f>
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="X6" s="5">
         <f ca="1">'base behaviour'!X6*RANDBETWEEN(75,100)/100</f>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="Y6" s="5">
         <f ca="1">'base behaviour'!Y6*RANDBETWEEN(75,100)/100</f>
-        <v>1.0101</v>
+        <v>0.93240000000000012</v>
       </c>
       <c r="Z6" s="5">
         <f ca="1">'base behaviour'!Z6*RANDBETWEEN(75,100)/100</f>
@@ -7031,48 +7031,48 @@
       </c>
       <c r="AA6" s="5">
         <f ca="1">'base behaviour'!AA6*RANDBETWEEN(75,100)/100</f>
-        <v>1.3171999999999999</v>
+        <v>1.3319999999999999</v>
       </c>
       <c r="AB6" s="5">
         <f ca="1">'base behaviour'!AB6*RANDBETWEEN(75,100)/100</f>
-        <v>1.2387999999999999</v>
+        <v>1.3039999999999998</v>
       </c>
       <c r="AC6" s="5">
         <f ca="1">'base behaviour'!AC6*RANDBETWEEN(75,100)/100</f>
-        <v>0.92819999999999991</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="AD6" s="5">
         <f ca="1">'base behaviour'!AD6*RANDBETWEEN(75,100)/100</f>
-        <v>0.78</v>
+        <v>0.86</v>
       </c>
       <c r="AE6" s="5">
         <f ca="1">'base behaviour'!AE6*RANDBETWEEN(75,100)/100</f>
-        <v>0.97749999999999981</v>
+        <v>1.0694999999999999</v>
       </c>
       <c r="AF6" s="5">
         <f ca="1">'base behaviour'!AF6*RANDBETWEEN(75,100)/100</f>
-        <v>0.92130000000000012</v>
+        <v>0.93240000000000012</v>
       </c>
       <c r="AG6" s="5">
         <f ca="1">'base behaviour'!AG6*RANDBETWEEN(75,100)/100</f>
-        <v>1.2348000000000001</v>
+        <v>1.0835999999999999</v>
       </c>
       <c r="AH6" s="5">
         <f ca="1">'base behaviour'!AH6*RANDBETWEEN(75,100)/100</f>
-        <v>1.4356</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="AI6" s="5">
         <f ca="1">'base behaviour'!AI6*RANDBETWEEN(75,100)/100</f>
-        <v>1.4995999999999998</v>
+        <v>1.4017999999999997</v>
       </c>
       <c r="AJ6" s="5">
         <f ca="1">'base behaviour'!AJ6*RANDBETWEEN(75,100)/100</f>
-        <v>0.92819999999999991</v>
+        <v>1.1661999999999999</v>
       </c>
       <c r="AK6" s="5"/>
       <c r="AL6" s="5">
         <f ca="1">SUM(B6:AK6)</f>
-        <v>31.617500000000003</v>
+        <v>31.889300000000002</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -7081,127 +7081,127 @@
       </c>
       <c r="B7" s="5">
         <f ca="1">'base behaviour'!B7*RANDBETWEEN(75,100)/100</f>
-        <v>0.93</v>
+        <v>0.87</v>
       </c>
       <c r="C7" s="5">
         <f ca="1">'base behaviour'!C7*RANDBETWEEN(75,100)/100</f>
-        <v>0.87399999999999989</v>
+        <v>0.90849999999999997</v>
       </c>
       <c r="D7" s="5">
         <f ca="1">'base behaviour'!D7*RANDBETWEEN(75,100)/100</f>
-        <v>0.85470000000000013</v>
+        <v>0.87690000000000012</v>
       </c>
       <c r="E7" s="5">
         <f ca="1">'base behaviour'!E7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1970000000000001</v>
+        <v>0.99540000000000006</v>
       </c>
       <c r="F7" s="5">
         <f ca="1">'base behaviour'!F7*RANDBETWEEN(75,100)/100</f>
-        <v>1.258</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="G7" s="5">
         <f ca="1">'base behaviour'!G7*RANDBETWEEN(75,100)/100</f>
-        <v>1.2550999999999999</v>
+        <v>1.3039999999999998</v>
       </c>
       <c r="H7" s="5">
         <f ca="1">'base behaviour'!H7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1305000000000001</v>
+        <v>1.1186</v>
       </c>
       <c r="I7" s="5">
         <f ca="1">'base behaviour'!I7*RANDBETWEEN(75,100)/100</f>
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="J7" s="5">
         <f ca="1">'base behaviour'!J7*RANDBETWEEN(75,100)/100</f>
-        <v>0.94299999999999995</v>
+        <v>1.1154999999999999</v>
       </c>
       <c r="K7" s="5">
         <f ca="1">'base behaviour'!K7*RANDBETWEEN(75,100)/100</f>
-        <v>0.84360000000000013</v>
+        <v>0.89910000000000012</v>
       </c>
       <c r="L7" s="5">
         <f ca="1">'base behaviour'!L7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1718000000000002</v>
+        <v>1.0332000000000001</v>
       </c>
       <c r="M7" s="5">
         <f ca="1">'base behaviour'!M7*RANDBETWEEN(75,100)/100</f>
-        <v>1.4652000000000001</v>
+        <v>1.1840000000000002</v>
       </c>
       <c r="N7" s="5">
         <f ca="1">'base behaviour'!N7*RANDBETWEEN(75,100)/100</f>
-        <v>1.3854999999999997</v>
+        <v>1.5159</v>
       </c>
       <c r="O7" s="5">
         <f ca="1">'base behaviour'!O7*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.1780999999999999</v>
       </c>
       <c r="P7" s="5">
         <f ca="1">'base behaviour'!P7*RANDBETWEEN(75,100)/100</f>
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="5">
         <f ca="1">'base behaviour'!Q7*RANDBETWEEN(75,100)/100</f>
-        <v>1.0349999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="R7" s="5">
         <f ca="1">'base behaviour'!R7*RANDBETWEEN(75,100)/100</f>
-        <v>0.97680000000000011</v>
+        <v>0.98790000000000011</v>
       </c>
       <c r="S7" s="5">
         <f ca="1">'base behaviour'!S7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1466000000000001</v>
+        <v>1.2473999999999998</v>
       </c>
       <c r="T7" s="5">
         <f ca="1">'base behaviour'!T7*RANDBETWEEN(75,100)/100</f>
-        <v>1.2875999999999999</v>
+        <v>1.2727999999999999</v>
       </c>
       <c r="U7" s="5">
         <f ca="1">'base behaviour'!U7*RANDBETWEEN(75,100)/100</f>
-        <v>1.4017999999999997</v>
+        <v>1.63</v>
       </c>
       <c r="V7" s="5">
         <f ca="1">'base behaviour'!V7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1186</v>
+        <v>1.1661999999999999</v>
       </c>
       <c r="W7" s="5">
         <f ca="1">'base behaviour'!W7*RANDBETWEEN(75,100)/100</f>
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="X7" s="5">
         <f ca="1">'base behaviour'!X7*RANDBETWEEN(75,100)/100</f>
-        <v>0.9544999999999999</v>
+        <v>1.081</v>
       </c>
       <c r="Y7" s="5">
         <f ca="1">'base behaviour'!Y7*RANDBETWEEN(75,100)/100</f>
-        <v>1.0989000000000002</v>
+        <v>0.92130000000000012</v>
       </c>
       <c r="Z7" s="5">
         <f ca="1">'base behaviour'!Z7*RANDBETWEEN(75,100)/100</f>
-        <v>1.008</v>
+        <v>1.071</v>
       </c>
       <c r="AA7" s="5">
         <f ca="1">'base behaviour'!AA7*RANDBETWEEN(75,100)/100</f>
-        <v>1.4652000000000001</v>
+        <v>1.4356</v>
       </c>
       <c r="AB7" s="5">
         <f ca="1">'base behaviour'!AB7*RANDBETWEEN(75,100)/100</f>
-        <v>1.5648</v>
+        <v>1.4017999999999997</v>
       </c>
       <c r="AC7" s="5">
         <f ca="1">'base behaviour'!AC7*RANDBETWEEN(75,100)/100</f>
-        <v>0.9163</v>
+        <v>0.98769999999999991</v>
       </c>
       <c r="AD7" s="5">
         <f ca="1">'base behaviour'!AD7*RANDBETWEEN(75,100)/100</f>
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
       <c r="AE7" s="5">
         <f ca="1">'base behaviour'!AE7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1154999999999999</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="AF7" s="5">
         <f ca="1">'base behaviour'!AF7*RANDBETWEEN(75,100)/100</f>
-        <v>1.1100000000000001</v>
+        <v>0.99900000000000011</v>
       </c>
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
@@ -7210,7 +7210,7 @@
       <c r="AK7" s="5"/>
       <c r="AL7" s="5">
         <f ca="1">SUM(B7:AK7)</f>
-        <v>34.058099999999996</v>
+        <v>34.609700000000004</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7222,79 +7222,79 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5">
         <f ca="1">'base behaviour'!E8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1088</v>
+        <v>1.2222</v>
       </c>
       <c r="F8" s="5">
         <f ca="1">'base behaviour'!F8*RANDBETWEEN(75,100)/100</f>
-        <v>1.2875999999999999</v>
+        <v>1.3615999999999999</v>
       </c>
       <c r="G8" s="5">
         <f ca="1">'base behaviour'!G8*RANDBETWEEN(75,100)/100</f>
-        <v>1.4180999999999999</v>
+        <v>1.6136999999999997</v>
       </c>
       <c r="H8" s="5">
         <f ca="1">'base behaviour'!H8*RANDBETWEEN(75,100)/100</f>
-        <v>0.99959999999999993</v>
+        <v>1.1067</v>
       </c>
       <c r="I8" s="5">
         <f ca="1">'base behaviour'!I8*RANDBETWEEN(75,100)/100</f>
-        <v>0.92</v>
+        <v>0.75</v>
       </c>
       <c r="J8" s="5">
         <f ca="1">'base behaviour'!J8*RANDBETWEEN(75,100)/100</f>
-        <v>0.96599999999999997</v>
+        <v>1.0465</v>
       </c>
       <c r="K8" s="5">
         <f ca="1">'base behaviour'!K8*RANDBETWEEN(75,100)/100</f>
-        <v>0.91020000000000012</v>
+        <v>0.85470000000000013</v>
       </c>
       <c r="L8" s="5">
         <f ca="1">'base behaviour'!L8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1592</v>
+        <v>1.1340000000000001</v>
       </c>
       <c r="M8" s="5">
         <f ca="1">'base behaviour'!M8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1840000000000002</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="N8" s="5">
         <f ca="1">'base behaviour'!N8*RANDBETWEEN(75,100)/100</f>
-        <v>1.2550999999999999</v>
+        <v>1.5973999999999997</v>
       </c>
       <c r="O8" s="5">
         <f ca="1">'base behaviour'!O8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1423999999999999</v>
+        <v>1.0948</v>
       </c>
       <c r="P8" s="5">
         <f ca="1">'base behaviour'!P8*RANDBETWEEN(75,100)/100</f>
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="Q8" s="5">
         <f ca="1">'base behaviour'!Q8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1499999999999999</v>
+        <v>1.0465</v>
       </c>
       <c r="R8" s="5">
         <f ca="1">'base behaviour'!R8*RANDBETWEEN(75,100)/100</f>
-        <v>1.0767000000000002</v>
+        <v>0.96570000000000011</v>
       </c>
       <c r="S8" s="5">
         <f ca="1">'base behaviour'!S8*RANDBETWEEN(75,100)/100</f>
-        <v>1.0458000000000001</v>
+        <v>1.0332000000000001</v>
       </c>
       <c r="T8" s="5">
         <f ca="1">'base behaviour'!T8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1395999999999999</v>
+        <v>1.3171999999999999</v>
       </c>
       <c r="U8" s="5">
         <f ca="1">'base behaviour'!U8*RANDBETWEEN(75,100)/100</f>
-        <v>1.5973999999999997</v>
+        <v>1.5810999999999999</v>
       </c>
       <c r="V8" s="5">
         <f ca="1">'base behaviour'!V8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1542999999999999</v>
+        <v>1.0353000000000001</v>
       </c>
       <c r="W8" s="5">
         <f ca="1">'base behaviour'!W8*RANDBETWEEN(75,100)/100</f>
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="X8" s="5">
         <f ca="1">'base behaviour'!X8*RANDBETWEEN(75,100)/100</f>
@@ -7302,50 +7302,50 @@
       </c>
       <c r="Y8" s="5">
         <f ca="1">'base behaviour'!Y8*RANDBETWEEN(75,100)/100</f>
-        <v>1.0101</v>
+        <v>0.97680000000000011</v>
       </c>
       <c r="Z8" s="5">
         <f ca="1">'base behaviour'!Z8*RANDBETWEEN(75,100)/100</f>
-        <v>1.26</v>
+        <v>1.1214</v>
       </c>
       <c r="AA8" s="5">
         <f ca="1">'base behaviour'!AA8*RANDBETWEEN(75,100)/100</f>
-        <v>1.2727999999999999</v>
+        <v>1.1543999999999999</v>
       </c>
       <c r="AB8" s="5">
         <f ca="1">'base behaviour'!AB8*RANDBETWEEN(75,100)/100</f>
-        <v>1.3529</v>
+        <v>1.2387999999999999</v>
       </c>
       <c r="AC8" s="5">
         <f ca="1">'base behaviour'!AC8*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.19</v>
       </c>
       <c r="AD8" s="5">
         <f ca="1">'base behaviour'!AD8*RANDBETWEEN(75,100)/100</f>
-        <v>0.99</v>
+        <v>0.84</v>
       </c>
       <c r="AE8" s="5">
         <f ca="1">'base behaviour'!AE8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1384999999999998</v>
+        <v>1.1039999999999999</v>
       </c>
       <c r="AF8" s="5">
         <f ca="1">'base behaviour'!AF8*RANDBETWEEN(75,100)/100</f>
-        <v>0.98790000000000011</v>
+        <v>0.91020000000000012</v>
       </c>
       <c r="AG8" s="5">
         <f ca="1">'base behaviour'!AG8*RANDBETWEEN(75,100)/100</f>
-        <v>1.2096</v>
+        <v>1.2348000000000001</v>
       </c>
       <c r="AH8" s="5">
         <f ca="1">'base behaviour'!AH8*RANDBETWEEN(75,100)/100</f>
-        <v>1.1395999999999999</v>
+        <v>1.2136</v>
       </c>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
       <c r="AK8" s="5"/>
       <c r="AL8" s="5">
         <f ca="1">SUM(B8:AK8)</f>
-        <v>33.737800000000007</v>
+        <v>33.961300000000001</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7359,15 +7359,15 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5">
         <f ca="1">'base behaviour'!G9*RANDBETWEEN(75,100)/100</f>
-        <v>1.3692</v>
+        <v>1.63</v>
       </c>
       <c r="H9" s="5">
         <f ca="1">'base behaviour'!H9*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.0114999999999998</v>
       </c>
       <c r="I9" s="5">
         <f ca="1">'base behaviour'!I9*RANDBETWEEN(75,100)/100</f>
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="J9" s="5">
         <f ca="1">'base behaviour'!J9*RANDBETWEEN(75,100)/100</f>
@@ -7375,115 +7375,115 @@
       </c>
       <c r="K9" s="5">
         <f ca="1">'base behaviour'!K9*RANDBETWEEN(75,100)/100</f>
-        <v>0.92130000000000012</v>
+        <v>0.87690000000000012</v>
       </c>
       <c r="L9" s="5">
         <f ca="1">'base behaviour'!L9*RANDBETWEEN(75,100)/100</f>
-        <v>1.071</v>
+        <v>1.0584</v>
       </c>
       <c r="M9" s="5">
         <f ca="1">'base behaviour'!M9*RANDBETWEEN(75,100)/100</f>
-        <v>1.1100000000000001</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="N9" s="5">
         <f ca="1">'base behaviour'!N9*RANDBETWEEN(75,100)/100</f>
-        <v>1.6136999999999997</v>
+        <v>1.3692</v>
       </c>
       <c r="O9" s="5">
         <f ca="1">'base behaviour'!O9*RANDBETWEEN(75,100)/100</f>
-        <v>1.1423999999999999</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="P9" s="5">
         <f ca="1">'base behaviour'!P9*RANDBETWEEN(75,100)/100</f>
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="Q9" s="5">
         <f ca="1">'base behaviour'!Q9*RANDBETWEEN(75,100)/100</f>
-        <v>0.94299999999999995</v>
+        <v>1.0234999999999999</v>
       </c>
       <c r="R9" s="5">
         <f ca="1">'base behaviour'!R9*RANDBETWEEN(75,100)/100</f>
-        <v>0.97680000000000011</v>
+        <v>1.0545</v>
       </c>
       <c r="S9" s="5">
         <f ca="1">'base behaviour'!S9*RANDBETWEEN(75,100)/100</f>
-        <v>1.1466000000000001</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="T9" s="5">
         <f ca="1">'base behaviour'!T9*RANDBETWEEN(75,100)/100</f>
-        <v>1.4356</v>
+        <v>1.1840000000000002</v>
       </c>
       <c r="U9" s="5">
         <f ca="1">'base behaviour'!U9*RANDBETWEEN(75,100)/100</f>
-        <v>1.5973999999999997</v>
+        <v>1.3692</v>
       </c>
       <c r="V9" s="5">
         <f ca="1">'base behaviour'!V9*RANDBETWEEN(75,100)/100</f>
-        <v>1.0471999999999999</v>
+        <v>0.9163</v>
       </c>
       <c r="W9" s="5">
         <f ca="1">'base behaviour'!W9*RANDBETWEEN(75,100)/100</f>
-        <v>0.77</v>
+        <v>0.94</v>
       </c>
       <c r="X9" s="5">
         <f ca="1">'base behaviour'!X9*RANDBETWEEN(75,100)/100</f>
-        <v>0.87399999999999989</v>
+        <v>0.88549999999999995</v>
       </c>
       <c r="Y9" s="5">
         <f ca="1">'base behaviour'!Y9*RANDBETWEEN(75,100)/100</f>
-        <v>1.0212000000000001</v>
+        <v>1.0545</v>
       </c>
       <c r="Z9" s="5">
         <f ca="1">'base behaviour'!Z9*RANDBETWEEN(75,100)/100</f>
-        <v>1.0584</v>
+        <v>1.1592</v>
       </c>
       <c r="AA9" s="5">
         <f ca="1">'base behaviour'!AA9*RANDBETWEEN(75,100)/100</f>
-        <v>1.4059999999999999</v>
+        <v>1.4503999999999999</v>
       </c>
       <c r="AB9" s="5">
         <f ca="1">'base behaviour'!AB9*RANDBETWEEN(75,100)/100</f>
-        <v>1.5485</v>
+        <v>1.3529</v>
       </c>
       <c r="AC9" s="5">
         <f ca="1">'base behaviour'!AC9*RANDBETWEEN(75,100)/100</f>
-        <v>1.1542999999999999</v>
+        <v>1.1186</v>
       </c>
       <c r="AD9" s="5">
         <f ca="1">'base behaviour'!AD9*RANDBETWEEN(75,100)/100</f>
-        <v>0.94</v>
+        <v>0.82</v>
       </c>
       <c r="AE9" s="5">
         <f ca="1">'base behaviour'!AE9*RANDBETWEEN(75,100)/100</f>
-        <v>0.88549999999999995</v>
+        <v>1.081</v>
       </c>
       <c r="AF9" s="5">
         <f ca="1">'base behaviour'!AF9*RANDBETWEEN(75,100)/100</f>
-        <v>0.89910000000000012</v>
+        <v>0.84360000000000013</v>
       </c>
       <c r="AG9" s="5">
         <f ca="1">'base behaviour'!AG9*RANDBETWEEN(75,100)/100</f>
-        <v>0.95760000000000001</v>
+        <v>1.1970000000000001</v>
       </c>
       <c r="AH9" s="5">
         <f ca="1">'base behaviour'!AH9*RANDBETWEEN(75,100)/100</f>
-        <v>1.3171999999999999</v>
+        <v>1.2283999999999999</v>
       </c>
       <c r="AI9" s="5">
         <f ca="1">'base behaviour'!AI9*RANDBETWEEN(75,100)/100</f>
-        <v>1.3039999999999998</v>
+        <v>1.4995999999999998</v>
       </c>
       <c r="AJ9" s="5">
         <f ca="1">'base behaviour'!AJ9*RANDBETWEEN(75,100)/100</f>
-        <v>0.98769999999999991</v>
+        <v>1.0114999999999998</v>
       </c>
       <c r="AK9" s="5">
         <f ca="1">'base behaviour'!AK9*RANDBETWEEN(75,100)/100</f>
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
       <c r="AL9" s="5">
         <f ca="1">SUM(B9:AK9)</f>
-        <v>34.2468</v>
+        <v>34.127399999999994</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7492,127 +7492,127 @@
       </c>
       <c r="B10" s="5">
         <f ca="1">'base behaviour'!B10*RANDBETWEEN(75,100)/100</f>
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="C10" s="5">
         <f ca="1">'base behaviour'!C10*RANDBETWEEN(75,100)/100</f>
-        <v>0.87399999999999989</v>
+        <v>0.97749999999999981</v>
       </c>
       <c r="D10" s="5">
         <f ca="1">'base behaviour'!D10*RANDBETWEEN(75,100)/100</f>
-        <v>0.97680000000000011</v>
+        <v>1.0101</v>
       </c>
       <c r="E10" s="5">
         <f ca="1">'base behaviour'!E10*RANDBETWEEN(75,100)/100</f>
-        <v>1.2348000000000001</v>
+        <v>0.97019999999999995</v>
       </c>
       <c r="F10" s="5">
         <f ca="1">'base behaviour'!F10*RANDBETWEEN(75,100)/100</f>
-        <v>1.4503999999999999</v>
+        <v>1.4059999999999999</v>
       </c>
       <c r="G10" s="5">
         <f ca="1">'base behaviour'!G10*RANDBETWEEN(75,100)/100</f>
-        <v>1.3039999999999998</v>
+        <v>1.4180999999999999</v>
       </c>
       <c r="H10" s="5">
         <f ca="1">'base behaviour'!H10*RANDBETWEEN(75,100)/100</f>
-        <v>1.1661999999999999</v>
+        <v>1.071</v>
       </c>
       <c r="I10" s="5">
         <f ca="1">'base behaviour'!I10*RANDBETWEEN(75,100)/100</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J10" s="5">
         <f ca="1">'base behaviour'!J10*RANDBETWEEN(75,100)/100</f>
-        <v>0.97749999999999981</v>
+        <v>0.89699999999999991</v>
       </c>
       <c r="K10" s="5">
         <f ca="1">'base behaviour'!K10*RANDBETWEEN(75,100)/100</f>
-        <v>1.0878000000000001</v>
+        <v>0.91020000000000012</v>
       </c>
       <c r="L10" s="5">
         <f ca="1">'base behaviour'!L10*RANDBETWEEN(75,100)/100</f>
-        <v>1.1592</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="M10" s="5">
         <f ca="1">'base behaviour'!M10*RANDBETWEEN(75,100)/100</f>
-        <v>1.1840000000000002</v>
+        <v>1.1248</v>
       </c>
       <c r="N10" s="5">
         <f ca="1">'base behaviour'!N10*RANDBETWEEN(75,100)/100</f>
-        <v>1.4180999999999999</v>
+        <v>1.2224999999999999</v>
       </c>
       <c r="O10" s="5">
         <f ca="1">'base behaviour'!O10*RANDBETWEEN(75,100)/100</f>
-        <v>0.98769999999999991</v>
+        <v>1.1186</v>
       </c>
       <c r="P10" s="5">
         <f ca="1">'base behaviour'!P10*RANDBETWEEN(75,100)/100</f>
-        <v>0.75</v>
+        <v>0.89</v>
       </c>
       <c r="Q10" s="5">
         <f ca="1">'base behaviour'!Q10*RANDBETWEEN(75,100)/100</f>
-        <v>0.89699999999999991</v>
+        <v>1.0465</v>
       </c>
       <c r="R10" s="5">
         <f ca="1">'base behaviour'!R10*RANDBETWEEN(75,100)/100</f>
-        <v>0.97680000000000011</v>
+        <v>1.0545</v>
       </c>
       <c r="S10" s="5">
         <f ca="1">'base behaviour'!S10*RANDBETWEEN(75,100)/100</f>
-        <v>1.1592</v>
+        <v>1.008</v>
       </c>
       <c r="T10" s="5">
         <f ca="1">'base behaviour'!T10*RANDBETWEEN(75,100)/100</f>
-        <v>1.1692</v>
+        <v>1.2727999999999999</v>
       </c>
       <c r="U10" s="5">
         <f ca="1">'base behaviour'!U10*RANDBETWEEN(75,100)/100</f>
-        <v>1.4343999999999999</v>
+        <v>1.3692</v>
       </c>
       <c r="V10" s="5">
         <f ca="1">'base behaviour'!V10*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.1542999999999999</v>
       </c>
       <c r="W10" s="5">
         <f ca="1">'base behaviour'!W10*RANDBETWEEN(75,100)/100</f>
-        <v>0.89</v>
+        <v>0.98</v>
       </c>
       <c r="X10" s="5">
         <f ca="1">'base behaviour'!X10*RANDBETWEEN(75,100)/100</f>
-        <v>0.96599999999999997</v>
+        <v>0.9544999999999999</v>
       </c>
       <c r="Y10" s="5">
         <f ca="1">'base behaviour'!Y10*RANDBETWEEN(75,100)/100</f>
-        <v>0.94350000000000012</v>
+        <v>0.83250000000000013</v>
       </c>
       <c r="Z10" s="5">
         <f ca="1">'base behaviour'!Z10*RANDBETWEEN(75,100)/100</f>
-        <v>1.008</v>
+        <v>1.26</v>
       </c>
       <c r="AA10" s="5">
         <f ca="1">'base behaviour'!AA10*RANDBETWEEN(75,100)/100</f>
-        <v>1.258</v>
+        <v>1.48</v>
       </c>
       <c r="AB10" s="5">
         <f ca="1">'base behaviour'!AB10*RANDBETWEEN(75,100)/100</f>
-        <v>1.5322</v>
+        <v>1.3854999999999997</v>
       </c>
       <c r="AC10" s="5">
         <f ca="1">'base behaviour'!AC10*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.1542999999999999</v>
       </c>
       <c r="AD10" s="5">
         <f ca="1">'base behaviour'!AD10*RANDBETWEEN(75,100)/100</f>
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="AE10" s="5">
         <f ca="1">'base behaviour'!AE10*RANDBETWEEN(75,100)/100</f>
-        <v>1.0004999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AF10" s="5">
         <f ca="1">'base behaviour'!AF10*RANDBETWEEN(75,100)/100</f>
-        <v>0.87690000000000012</v>
+        <v>1.0434000000000001</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
@@ -7621,7 +7621,7 @@
       <c r="AK10" s="5"/>
       <c r="AL10" s="5">
         <f ca="1">SUM(B10:AK10)</f>
-        <v>33.282399999999996</v>
+        <v>33.546500000000002</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7633,35 +7633,35 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5">
         <f ca="1">'base behaviour'!E11*RANDBETWEEN(75,100)/100</f>
-        <v>0.97019999999999995</v>
+        <v>1.1592</v>
       </c>
       <c r="F11" s="5">
         <f ca="1">'base behaviour'!F11*RANDBETWEEN(75,100)/100</f>
-        <v>1.4652000000000001</v>
+        <v>1.3024</v>
       </c>
       <c r="G11" s="5">
         <f ca="1">'base behaviour'!G11*RANDBETWEEN(75,100)/100</f>
-        <v>1.2713999999999999</v>
+        <v>1.4506999999999999</v>
       </c>
       <c r="H11" s="5">
         <f ca="1">'base behaviour'!H11*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.1186</v>
       </c>
       <c r="I11" s="5">
         <f ca="1">'base behaviour'!I11*RANDBETWEEN(75,100)/100</f>
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="J11" s="5">
         <f ca="1">'base behaviour'!J11*RANDBETWEEN(75,100)/100</f>
-        <v>0.93149999999999988</v>
+        <v>1.1384999999999998</v>
       </c>
       <c r="K11" s="5">
         <f ca="1">'base behaviour'!K11*RANDBETWEEN(75,100)/100</f>
-        <v>1.0212000000000001</v>
+        <v>0.86580000000000013</v>
       </c>
       <c r="L11" s="5">
         <f ca="1">'base behaviour'!L11*RANDBETWEEN(75,100)/100</f>
-        <v>1.1466000000000001</v>
+        <v>1.1088</v>
       </c>
       <c r="M11" s="5">
         <f ca="1">'base behaviour'!M11*RANDBETWEEN(75,100)/100</f>
@@ -7669,94 +7669,94 @@
       </c>
       <c r="N11" s="5">
         <f ca="1">'base behaviour'!N11*RANDBETWEEN(75,100)/100</f>
-        <v>1.3039999999999998</v>
+        <v>1.4343999999999999</v>
       </c>
       <c r="O11" s="5">
         <f ca="1">'base behaviour'!O11*RANDBETWEEN(75,100)/100</f>
-        <v>1.1661999999999999</v>
+        <v>0.9758</v>
       </c>
       <c r="P11" s="5">
         <f ca="1">'base behaviour'!P11*RANDBETWEEN(75,100)/100</f>
-        <v>0.97</v>
+        <v>0.87</v>
       </c>
       <c r="Q11" s="5">
         <f ca="1">'base behaviour'!Q11*RANDBETWEEN(75,100)/100</f>
-        <v>1.0465</v>
+        <v>1.1154999999999999</v>
       </c>
       <c r="R11" s="5">
         <f ca="1">'base behaviour'!R11*RANDBETWEEN(75,100)/100</f>
-        <v>0.95460000000000012</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="S11" s="5">
         <f ca="1">'base behaviour'!S11*RANDBETWEEN(75,100)/100</f>
-        <v>3.6666000000000003</v>
+        <v>3.1374</v>
       </c>
       <c r="T11" s="5">
         <f ca="1">'base behaviour'!T11*RANDBETWEEN(75,100)/100</f>
-        <v>4.0404</v>
+        <v>4.0847999999999995</v>
       </c>
       <c r="U11" s="5">
         <f ca="1">'base behaviour'!U11*RANDBETWEEN(75,100)/100</f>
-        <v>1.5810999999999999</v>
+        <v>1.4832999999999998</v>
       </c>
       <c r="V11" s="5">
         <f ca="1">'base behaviour'!V11*RANDBETWEEN(75,100)/100</f>
-        <v>0.9758</v>
+        <v>0.89249999999999996</v>
       </c>
       <c r="W11" s="5">
         <f ca="1">'base behaviour'!W11*RANDBETWEEN(75,100)/100</f>
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="X11" s="5">
         <f ca="1">'base behaviour'!X11*RANDBETWEEN(75,100)/100</f>
-        <v>1.0465</v>
+        <v>1.0119999999999998</v>
       </c>
       <c r="Y11" s="5">
         <f ca="1">'base behaviour'!Y11*RANDBETWEEN(75,100)/100</f>
-        <v>0.99900000000000011</v>
+        <v>0.92130000000000012</v>
       </c>
       <c r="Z11" s="5">
         <f ca="1">'base behaviour'!Z11*RANDBETWEEN(75,100)/100</f>
-        <v>1.1718000000000002</v>
+        <v>1.1214</v>
       </c>
       <c r="AA11" s="5">
         <f ca="1">'base behaviour'!AA11*RANDBETWEEN(75,100)/100</f>
-        <v>1.48</v>
+        <v>1.2727999999999999</v>
       </c>
       <c r="AB11" s="5">
         <f ca="1">'base behaviour'!AB11*RANDBETWEEN(75,100)/100</f>
-        <v>1.2224999999999999</v>
+        <v>1.3203</v>
       </c>
       <c r="AC11" s="5">
         <f ca="1">'base behaviour'!AC11*RANDBETWEEN(75,100)/100</f>
-        <v>1.0590999999999999</v>
+        <v>1.071</v>
       </c>
       <c r="AD11" s="5">
         <f ca="1">'base behaviour'!AD11*RANDBETWEEN(75,100)/100</f>
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="AE11" s="5">
         <f ca="1">'base behaviour'!AE11*RANDBETWEEN(75,100)/100</f>
-        <v>0.90849999999999997</v>
+        <v>0.89699999999999991</v>
       </c>
       <c r="AF11" s="5">
         <f ca="1">'base behaviour'!AF11*RANDBETWEEN(75,100)/100</f>
-        <v>1.0767000000000002</v>
+        <v>1.0101</v>
       </c>
       <c r="AG11" s="5">
         <f ca="1">'base behaviour'!AG11*RANDBETWEEN(75,100)/100</f>
-        <v>1.1843999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="AH11" s="5">
         <f ca="1">'base behaviour'!AH11*RANDBETWEEN(75,100)/100</f>
-        <v>1.3024</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
       <c r="AK11" s="5"/>
       <c r="AL11" s="5">
         <f ca="1">SUM(B11:AK11)</f>
-        <v>38.828299999999992</v>
+        <v>38.620399999999989</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -7770,131 +7770,131 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5">
         <f ca="1">'base behaviour'!G12*RANDBETWEEN(75,100)/100</f>
-        <v>1.3529</v>
+        <v>1.5648</v>
       </c>
       <c r="H12" s="5">
         <f ca="1">'base behaviour'!H12*RANDBETWEEN(75,100)/100</f>
-        <v>0.9758</v>
+        <v>0.92819999999999991</v>
       </c>
       <c r="I12" s="5">
         <f ca="1">'base behaviour'!I12*RANDBETWEEN(75,100)/100</f>
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="J12" s="5">
         <f ca="1">'base behaviour'!J12*RANDBETWEEN(75,100)/100</f>
-        <v>0.93149999999999988</v>
+        <v>1.0694999999999999</v>
       </c>
       <c r="K12" s="5">
         <f ca="1">'base behaviour'!K12*RANDBETWEEN(75,100)/100</f>
-        <v>0.95460000000000012</v>
+        <v>0.84360000000000013</v>
       </c>
       <c r="L12" s="5">
         <f ca="1">'base behaviour'!L12*RANDBETWEEN(75,100)/100</f>
-        <v>0.95760000000000001</v>
+        <v>1.2473999999999998</v>
       </c>
       <c r="M12" s="5">
         <f ca="1">'base behaviour'!M12*RANDBETWEEN(75,100)/100</f>
-        <v>1.3319999999999999</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="N12" s="5">
         <f ca="1">'base behaviour'!N12*RANDBETWEEN(75,100)/100</f>
-        <v>1.5485</v>
+        <v>1.5648</v>
       </c>
       <c r="O12" s="5">
         <f ca="1">'base behaviour'!O12*RANDBETWEEN(75,100)/100</f>
-        <v>1.071</v>
+        <v>1.1661999999999999</v>
       </c>
       <c r="P12" s="5">
         <f ca="1">'base behaviour'!P12*RANDBETWEEN(75,100)/100</f>
-        <v>0.82</v>
+        <v>0.94</v>
       </c>
       <c r="Q12" s="5">
         <f ca="1">'base behaviour'!Q12*RANDBETWEEN(75,100)/100</f>
-        <v>0.93149999999999988</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="R12" s="5">
         <f ca="1">'base behaviour'!R12*RANDBETWEEN(75,100)/100</f>
-        <v>0.85470000000000013</v>
+        <v>1.0656000000000001</v>
       </c>
       <c r="S12" s="5">
         <f ca="1">'base behaviour'!S12*RANDBETWEEN(75,100)/100</f>
-        <v>1.2348000000000001</v>
+        <v>1.0332000000000001</v>
       </c>
       <c r="T12" s="5">
         <f ca="1">'base behaviour'!T12*RANDBETWEEN(75,100)/100</f>
-        <v>1.3171999999999999</v>
+        <v>1.2283999999999999</v>
       </c>
       <c r="U12" s="5">
         <f ca="1">'base behaviour'!U12*RANDBETWEEN(75,100)/100</f>
-        <v>1.5810999999999999</v>
+        <v>1.3854999999999997</v>
       </c>
       <c r="V12" s="5">
         <f ca="1">'base behaviour'!V12*RANDBETWEEN(75,100)/100</f>
-        <v>1.0233999999999999</v>
+        <v>1.1542999999999999</v>
       </c>
       <c r="W12" s="5">
         <f ca="1">'base behaviour'!W12*RANDBETWEEN(75,100)/100</f>
-        <v>0.76</v>
+        <v>0.93</v>
       </c>
       <c r="X12" s="5">
         <f ca="1">'base behaviour'!X12*RANDBETWEEN(75,100)/100</f>
-        <v>0.87399999999999989</v>
+        <v>1.1384999999999998</v>
       </c>
       <c r="Y12" s="5">
         <f ca="1">'base behaviour'!Y12*RANDBETWEEN(75,100)/100</f>
-        <v>0.95460000000000012</v>
+        <v>1.0878000000000001</v>
       </c>
       <c r="Z12" s="5">
         <f ca="1">'base behaviour'!Z12*RANDBETWEEN(75,100)/100</f>
-        <v>0.99540000000000006</v>
+        <v>1.2473999999999998</v>
       </c>
       <c r="AA12" s="5">
         <f ca="1">'base behaviour'!AA12*RANDBETWEEN(75,100)/100</f>
-        <v>1.3468</v>
+        <v>1.4059999999999999</v>
       </c>
       <c r="AB12" s="5">
         <f ca="1">'base behaviour'!AB12*RANDBETWEEN(75,100)/100</f>
-        <v>1.3529</v>
+        <v>1.4343999999999999</v>
       </c>
       <c r="AC12" s="5">
         <f ca="1">'base behaviour'!AC12*RANDBETWEEN(75,100)/100</f>
-        <v>1.1780999999999999</v>
+        <v>1.1067</v>
       </c>
       <c r="AD12" s="5">
         <f ca="1">'base behaviour'!AD12*RANDBETWEEN(75,100)/100</f>
-        <v>0.95</v>
+        <v>0.79</v>
       </c>
       <c r="AE12" s="5">
         <f ca="1">'base behaviour'!AE12*RANDBETWEEN(75,100)/100</f>
-        <v>0.96599999999999997</v>
+        <v>1.1384999999999998</v>
       </c>
       <c r="AF12" s="5">
         <f ca="1">'base behaviour'!AF12*RANDBETWEEN(75,100)/100</f>
-        <v>1.0767000000000002</v>
+        <v>0.94350000000000012</v>
       </c>
       <c r="AG12" s="5">
         <f ca="1">'base behaviour'!AG12*RANDBETWEEN(75,100)/100</f>
-        <v>1.1340000000000001</v>
+        <v>1.008</v>
       </c>
       <c r="AH12" s="5">
         <f ca="1">'base behaviour'!AH12*RANDBETWEEN(75,100)/100</f>
-        <v>1.4652000000000001</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="AI12" s="5">
         <f ca="1">'base behaviour'!AI12*RANDBETWEEN(75,100)/100</f>
-        <v>1.4017999999999997</v>
+        <v>1.5648</v>
       </c>
       <c r="AJ12" s="5">
         <f ca="1">'base behaviour'!AJ12*RANDBETWEEN(75,100)/100</f>
-        <v>1.0948</v>
+        <v>1.071</v>
       </c>
       <c r="AK12" s="5">
         <f ca="1">'base behaviour'!AK12*RANDBETWEEN(75,100)/100</f>
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="AL12" s="5">
         <f ca="1">SUM(B12:AK12)</f>
-        <v>34.306899999999992</v>
+        <v>35.594699999999989</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -7903,123 +7903,123 @@
       </c>
       <c r="B13" s="5">
         <f ca="1">'base behaviour'!B13*RANDBETWEEN(75,100)/100</f>
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="C13" s="5">
         <f ca="1">'base behaviour'!C13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0924999999999998</v>
+        <v>1.0694999999999999</v>
       </c>
       <c r="D13" s="5">
         <f ca="1">'base behaviour'!D13*RANDBETWEEN(75,100)/100</f>
-        <v>0.93240000000000012</v>
+        <v>1.0989000000000002</v>
       </c>
       <c r="E13" s="5">
         <f ca="1">'base behaviour'!E13*RANDBETWEEN(75,100)/100</f>
-        <v>1.1970000000000001</v>
+        <v>1.0206</v>
       </c>
       <c r="F13" s="5">
         <f ca="1">'base behaviour'!F13*RANDBETWEEN(75,100)/100</f>
-        <v>1.4503999999999999</v>
+        <v>1.3319999999999999</v>
       </c>
       <c r="G13" s="5">
         <f ca="1">'base behaviour'!G13*RANDBETWEEN(75,100)/100</f>
-        <v>1.3366</v>
+        <v>1.2713999999999999</v>
       </c>
       <c r="H13" s="5">
         <f ca="1">'base behaviour'!H13*RANDBETWEEN(75,100)/100</f>
-        <v>0.94009999999999994</v>
+        <v>1.1542999999999999</v>
       </c>
       <c r="I13" s="5">
         <f ca="1">'base behaviour'!I13*RANDBETWEEN(75,100)/100</f>
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
       <c r="J13" s="5">
         <f ca="1">'base behaviour'!J13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0234999999999999</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="K13" s="5">
         <f ca="1">'base behaviour'!K13*RANDBETWEEN(75,100)/100</f>
-        <v>0.99900000000000011</v>
+        <v>0.85470000000000013</v>
       </c>
       <c r="L13" s="5">
         <f ca="1">'base behaviour'!L13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0962000000000001</v>
+        <v>1.0835999999999999</v>
       </c>
       <c r="M13" s="5">
         <f ca="1">'base behaviour'!M13*RANDBETWEEN(75,100)/100</f>
-        <v>1.1987999999999999</v>
+        <v>1.1692</v>
       </c>
       <c r="N13" s="5">
         <f ca="1">'base behaviour'!N13*RANDBETWEEN(75,100)/100</f>
-        <v>1.4506999999999999</v>
+        <v>1.5159</v>
       </c>
       <c r="O13" s="5">
         <f ca="1">'base behaviour'!O13*RANDBETWEEN(75,100)/100</f>
-        <v>0.9163</v>
+        <v>1.1661999999999999</v>
       </c>
       <c r="P13" s="5">
         <f ca="1">'base behaviour'!P13*RANDBETWEEN(75,100)/100</f>
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="Q13" s="5">
         <f ca="1">'base behaviour'!Q13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0234999999999999</v>
+        <v>1.0694999999999999</v>
       </c>
       <c r="R13" s="5">
         <f ca="1">'base behaviour'!R13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0878000000000001</v>
+        <v>1.0545</v>
       </c>
       <c r="S13" s="5">
         <f ca="1">'base behaviour'!S13*RANDBETWEEN(75,100)/100</f>
-        <v>0.99540000000000006</v>
+        <v>1.0584</v>
       </c>
       <c r="T13" s="5">
         <f ca="1">'base behaviour'!T13*RANDBETWEEN(75,100)/100</f>
-        <v>1.4059999999999999</v>
+        <v>1.1395999999999999</v>
       </c>
       <c r="U13" s="5">
         <f ca="1">'base behaviour'!U13*RANDBETWEEN(75,100)/100</f>
-        <v>1.5810999999999999</v>
+        <v>1.5159</v>
       </c>
       <c r="V13" s="5">
         <f ca="1">'base behaviour'!V13*RANDBETWEEN(75,100)/100</f>
-        <v>1.1067</v>
+        <v>1.1661999999999999</v>
       </c>
       <c r="W13" s="5">
         <f ca="1">'base behaviour'!W13*RANDBETWEEN(75,100)/100</f>
-        <v>0.81</v>
+        <v>0.88</v>
       </c>
       <c r="X13" s="5">
         <f ca="1">'base behaviour'!X13*RANDBETWEEN(75,100)/100</f>
-        <v>1.081</v>
+        <v>0.90849999999999997</v>
       </c>
       <c r="Y13" s="5">
         <f ca="1">'base behaviour'!Y13*RANDBETWEEN(75,100)/100</f>
-        <v>1.0545</v>
+        <v>0.92130000000000012</v>
       </c>
       <c r="Z13" s="5">
         <f ca="1">'base behaviour'!Z13*RANDBETWEEN(75,100)/100</f>
-        <v>0.97019999999999995</v>
+        <v>1.1088</v>
       </c>
       <c r="AA13" s="5">
         <f ca="1">'base behaviour'!AA13*RANDBETWEEN(75,100)/100</f>
-        <v>1.4652000000000001</v>
+        <v>1.4207999999999998</v>
       </c>
       <c r="AB13" s="5">
         <f ca="1">'base behaviour'!AB13*RANDBETWEEN(75,100)/100</f>
-        <v>1.5485</v>
+        <v>1.4669999999999999</v>
       </c>
       <c r="AC13" s="5">
         <f ca="1">'base behaviour'!AC13*RANDBETWEEN(75,100)/100</f>
-        <v>0.95199999999999985</v>
+        <v>1.0353000000000001</v>
       </c>
       <c r="AD13" s="5">
         <f ca="1">'base behaviour'!AD13*RANDBETWEEN(75,100)/100</f>
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
       <c r="AE13" s="5">
         <f ca="1">'base behaviour'!AE13*RANDBETWEEN(75,100)/100</f>
-        <v>1.1499999999999999</v>
+        <v>0.88549999999999995</v>
       </c>
       <c r="AF13" s="5"/>
       <c r="AG13" s="5"/>
@@ -8029,7 +8029,7 @@
       <c r="AK13" s="5"/>
       <c r="AL13" s="5">
         <f ca="1">SUM(B13:AK13)</f>
-        <v>33.405399999999993</v>
+        <v>32.642599999999995</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -8040,134 +8040,134 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5">
         <f ca="1">'base behaviour'!D14*RANDBETWEEN(75,100)/100</f>
-        <v>0.93240000000000012</v>
+        <v>0.89910000000000012</v>
       </c>
       <c r="E14" s="5">
         <f ca="1">'base behaviour'!E14*RANDBETWEEN(75,100)/100</f>
-        <v>0.95760000000000001</v>
+        <v>1.1214</v>
       </c>
       <c r="F14" s="5">
         <f ca="1">'base behaviour'!F14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1543999999999999</v>
+        <v>1.2875999999999999</v>
       </c>
       <c r="G14" s="5">
         <f ca="1">'base behaviour'!G14*RANDBETWEEN(75,100)/100</f>
-        <v>1.3529</v>
+        <v>1.3854999999999997</v>
       </c>
       <c r="H14" s="5">
         <f ca="1">'base behaviour'!H14*RANDBETWEEN(75,100)/100</f>
-        <v>1.0590999999999999</v>
+        <v>1.1305000000000001</v>
       </c>
       <c r="I14" s="5">
         <f ca="1">'base behaviour'!I14*RANDBETWEEN(75,100)/100</f>
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="J14" s="5">
         <f ca="1">'base behaviour'!J14*RANDBETWEEN(75,100)/100</f>
-        <v>0.89699999999999991</v>
+        <v>0.88549999999999995</v>
       </c>
       <c r="K14" s="5">
         <f ca="1">'base behaviour'!K14*RANDBETWEEN(75,100)/100</f>
-        <v>0.83250000000000013</v>
+        <v>0.99900000000000011</v>
       </c>
       <c r="L14" s="5">
         <f ca="1">'base behaviour'!L14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1592</v>
+        <v>1.0458000000000001</v>
       </c>
       <c r="M14" s="5">
         <f ca="1">'base behaviour'!M14*RANDBETWEEN(75,100)/100</f>
-        <v>1.3615999999999999</v>
+        <v>1.1692</v>
       </c>
       <c r="N14" s="5">
         <f ca="1">'base behaviour'!N14*RANDBETWEEN(75,100)/100</f>
-        <v>1.5810999999999999</v>
+        <v>1.4506999999999999</v>
       </c>
       <c r="O14" s="5">
         <f ca="1">'base behaviour'!O14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1305000000000001</v>
+        <v>1.1423999999999999</v>
       </c>
       <c r="P14" s="5">
         <f ca="1">'base behaviour'!P14*RANDBETWEEN(75,100)/100</f>
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="Q14" s="5">
         <f ca="1">'base behaviour'!Q14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1499999999999999</v>
+        <v>1.1154999999999999</v>
       </c>
       <c r="R14" s="5">
         <f ca="1">'base behaviour'!R14*RANDBETWEEN(75,100)/100</f>
-        <v>0.88800000000000012</v>
+        <v>1.0323</v>
       </c>
       <c r="S14" s="5">
         <f ca="1">'base behaviour'!S14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1970000000000001</v>
+        <v>1.0835999999999999</v>
       </c>
       <c r="T14" s="5">
         <f ca="1">'base behaviour'!T14*RANDBETWEEN(75,100)/100</f>
-        <v>1.1987999999999999</v>
+        <v>1.3024</v>
       </c>
       <c r="U14" s="5">
         <f ca="1">'base behaviour'!U14*RANDBETWEEN(75,100)/100</f>
-        <v>2.6732</v>
+        <v>3.2273999999999994</v>
       </c>
       <c r="V14" s="5">
         <f ca="1">'base behaviour'!V14*RANDBETWEEN(75,100)/100</f>
-        <v>2.2372000000000001</v>
+        <v>2.3085999999999998</v>
       </c>
       <c r="W14" s="5">
         <f ca="1">'base behaviour'!W14*RANDBETWEEN(75,100)/100</f>
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="X14" s="5">
         <f ca="1">'base behaviour'!X14*RANDBETWEEN(75,100)/100</f>
-        <v>1.7479999999999998</v>
+        <v>2.1619999999999999</v>
       </c>
       <c r="Y14" s="5">
         <f ca="1">'base behaviour'!Y14*RANDBETWEEN(75,100)/100</f>
-        <v>1.8204000000000002</v>
+        <v>1.9980000000000002</v>
       </c>
       <c r="Z14" s="5">
         <f ca="1">'base behaviour'!Z14*RANDBETWEEN(75,100)/100</f>
-        <v>2.3436000000000003</v>
+        <v>1.9656</v>
       </c>
       <c r="AA14" s="5">
         <f ca="1">'base behaviour'!AA14*RANDBETWEEN(75,100)/100</f>
-        <v>2.4567999999999999</v>
+        <v>2.7527999999999997</v>
       </c>
       <c r="AB14" s="5">
         <f ca="1">'base behaviour'!AB14*RANDBETWEEN(75,100)/100</f>
-        <v>2.7709999999999995</v>
+        <v>2.9013999999999998</v>
       </c>
       <c r="AC14" s="5">
         <f ca="1">'base behaviour'!AC14*RANDBETWEEN(75,100)/100</f>
-        <v>1.9991999999999999</v>
+        <v>2.3085999999999998</v>
       </c>
       <c r="AD14" s="5">
         <f ca="1">'base behaviour'!AD14*RANDBETWEEN(75,100)/100</f>
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="AE14" s="5">
         <f ca="1">'base behaviour'!AE14*RANDBETWEEN(75,100)/100</f>
-        <v>2.0239999999999996</v>
+        <v>1.9549999999999996</v>
       </c>
       <c r="AF14" s="5">
         <f ca="1">'base behaviour'!AF14*RANDBETWEEN(75,100)/100</f>
-        <v>2.0868000000000002</v>
+        <v>1.9536000000000002</v>
       </c>
       <c r="AG14" s="5">
         <f ca="1">'base behaviour'!AG14*RANDBETWEEN(75,100)/100</f>
-        <v>2.0664000000000002</v>
+        <v>2.2176</v>
       </c>
       <c r="AH14" s="5">
         <f ca="1">'base behaviour'!AH14*RANDBETWEEN(75,100)/100</f>
-        <v>2.7527999999999997</v>
+        <v>2.516</v>
       </c>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
       <c r="AL14" s="5">
         <f ca="1">SUM(B14:AK14)</f>
-        <v>49.161500000000011</v>
+        <v>50.217099999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>